<commit_message>
all food and meal data from external JSON
</commit_message>
<xml_diff>
--- a/ExcelIntegration/data/calorie_table_with_codes.xlsx
+++ b/ExcelIntegration/data/calorie_table_with_codes.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sandbox\git\aadennis\PythonSandboxAA\ExcelIntegration\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F6EDEC-077C-42B7-AFD4-CFAFFE075304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-30828" yWindow="3684" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Food Items" sheetId="1" r:id="rId1"/>
     <sheet name="Meals" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
   <si>
     <t>Food Item</t>
   </si>
@@ -38,43 +44,34 @@
     <t>Frozen Bananas</t>
   </si>
   <si>
-    <t>Greek Yoghurt (plain, non-fat)</t>
+    <t>Lidl Greek Style Yoghurt (Full Fat)</t>
   </si>
   <si>
     <t>Brown Sugar (1 tbsp)</t>
   </si>
   <si>
-    <t>Brown Sugar (1 tsp)</t>
-  </si>
-  <si>
     <t>Semi-skimmed Milk (50 ml)</t>
   </si>
   <si>
+    <t>Honey</t>
+  </si>
+  <si>
+    <t>Homemade Vegetable Soup</t>
+  </si>
+  <si>
+    <t>Sourdough Bread</t>
+  </si>
+  <si>
+    <t>Butter</t>
+  </si>
+  <si>
+    <t>Nespresso coffee pod</t>
+  </si>
+  <si>
     <t>Semi-skimmed Milk (100 ml)</t>
   </si>
   <si>
-    <t>Sourdough Bread</t>
-  </si>
-  <si>
-    <t>Butter</t>
-  </si>
-  <si>
-    <t>Jam</t>
-  </si>
-  <si>
-    <t>Honey</t>
-  </si>
-  <si>
-    <t>Homemade Vegetable Soup</t>
-  </si>
-  <si>
-    <t>Full-Fat Milk</t>
-  </si>
-  <si>
-    <t>Peas</t>
-  </si>
-  <si>
-    <t>Lidl Greek Style Yoghurt (Full Fat)</t>
+    <t>Polish Wafer</t>
   </si>
   <si>
     <t>FSXX</t>
@@ -83,43 +80,34 @@
     <t>FBXX</t>
   </si>
   <si>
-    <t>GYPN</t>
+    <t>LGSY</t>
   </si>
   <si>
     <t>BS1T</t>
   </si>
   <si>
-    <t>BS12</t>
-  </si>
-  <si>
     <t>SM5M</t>
   </si>
   <si>
+    <t>HONE</t>
+  </si>
+  <si>
+    <t>HVSX</t>
+  </si>
+  <si>
+    <t>SBXX</t>
+  </si>
+  <si>
+    <t>BUTT</t>
+  </si>
+  <si>
+    <t>NCPX</t>
+  </si>
+  <si>
     <t>SM1M</t>
   </si>
   <si>
-    <t>SBXX</t>
-  </si>
-  <si>
-    <t>BUTT</t>
-  </si>
-  <si>
-    <t>JAMX</t>
-  </si>
-  <si>
-    <t>HONE</t>
-  </si>
-  <si>
-    <t>HVSX</t>
-  </si>
-  <si>
-    <t>FMXX</t>
-  </si>
-  <si>
-    <t>PEAS</t>
-  </si>
-  <si>
-    <t>LGSY</t>
+    <t>PWXX</t>
   </si>
   <si>
     <t>g</t>
@@ -128,16 +116,19 @@
     <t>tbsp</t>
   </si>
   <si>
-    <t>tsp</t>
-  </si>
-  <si>
     <t>ml</t>
   </si>
   <si>
+    <t>bowl</t>
+  </si>
+  <si>
     <t>slice</t>
   </si>
   <si>
-    <t>bowl</t>
+    <t>pod</t>
+  </si>
+  <si>
+    <t>wafer</t>
   </si>
   <si>
     <t>Meals</t>
@@ -173,11 +164,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,13 +251,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -304,7 +303,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -338,6 +337,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -372,9 +372,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -547,21 +548,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="37.7265625" customWidth="1"/>
+    <col min="2" max="2" width="6.7265625" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" customWidth="1"/>
+    <col min="4" max="4" width="7.7265625" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,259 +581,208 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E3">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E4">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E6">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8">
         <v>100</v>
       </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E9">
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E10">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E12">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14">
-        <v>200</v>
-      </c>
-      <c r="D14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15">
-        <v>100</v>
-      </c>
-      <c r="D15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16">
-        <v>100</v>
-      </c>
-      <c r="D16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16">
-        <v>126</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -839,24 +791,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -864,18 +825,18 @@
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -890,9 +851,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -907,12 +868,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -924,9 +885,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -941,12 +902,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5">
         <v>1.5</v>
@@ -958,12 +919,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -975,20 +936,20 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D12" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E12" s="5">
         <v>438</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>1</v>
       </c>
@@ -996,21 +957,21 @@
         <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1022,9 +983,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
@@ -1039,9 +1000,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
@@ -1056,12 +1017,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1073,12 +1034,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1090,12 +1051,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1107,9 +1068,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D23" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E23" s="5">
         <v>401</v>

</xml_diff>

<commit_message>
Fix food code in meals.json (should align with what the script generates)
</commit_message>
<xml_diff>
--- a/ExcelIntegration/data/calorie_table_with_codes.xlsx
+++ b/ExcelIntegration/data/calorie_table_with_codes.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sandbox\git\aadennis\PythonSandboxAA\ExcelIntegration\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F6EDEC-077C-42B7-AFD4-CFAFFE075304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="3684" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Food Items" sheetId="1" r:id="rId1"/>
     <sheet name="Meals" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t>Food Item</t>
   </si>
@@ -156,19 +150,16 @@
   </si>
   <si>
     <t>Not Found</t>
-  </si>
-  <si>
-    <t>PLWF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,21 +242,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -303,7 +286,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -337,7 +320,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -372,10 +354,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -548,23 +529,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.7265625" customWidth="1"/>
-    <col min="2" max="2" width="6.7265625" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" customWidth="1"/>
-    <col min="5" max="5" width="17.7265625" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -598,7 +577,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -615,7 +594,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -632,7 +611,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -649,7 +628,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -666,7 +645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -683,7 +662,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -700,7 +679,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -717,7 +696,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -734,7 +713,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -751,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -768,7 +747,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -791,33 +770,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -834,7 +804,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -851,7 +821,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -868,7 +838,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -885,7 +855,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -902,7 +872,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -919,7 +889,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -936,7 +906,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5">
       <c r="D12" s="4" t="s">
         <v>41</v>
       </c>
@@ -944,12 +914,12 @@
         <v>438</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
         <v>1</v>
       </c>
@@ -966,7 +936,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -983,7 +953,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1000,7 +970,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1017,7 +987,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1034,7 +1004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1051,29 +1021,29 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="D23" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E23" s="5">
-        <v>401</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>